<commit_message>
tissue specific GO visualizations
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis/GO_results_tissue/tissue_go_results.xlsx
+++ b/gene_ontology_analysis/GO_results_tissue/tissue_go_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporal gene/gene_ontology_analysis/GO_results_tissue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB19FC-B10E-7446-A9F1-A4A8CF1FB5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DE02A5-F4C0-D146-B349-554B2DFC6F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouse_Gene_Atlas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="309">
   <si>
     <t>Rank</t>
   </si>
@@ -846,6 +846,108 @@
   </si>
   <si>
     <t>['AGER']</t>
+  </si>
+  <si>
+    <t>Lung specific Gene</t>
+  </si>
+  <si>
+    <t>Correlation value in validation</t>
+  </si>
+  <si>
+    <t>FOXF2</t>
+  </si>
+  <si>
+    <t>ABCA3</t>
+  </si>
+  <si>
+    <t>ADAMTSL2</t>
+  </si>
+  <si>
+    <t>AGER</t>
+  </si>
+  <si>
+    <t>INMT</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.9423</t>
+  </si>
+  <si>
+    <t>0.7421</t>
+  </si>
+  <si>
+    <t>0.8393</t>
+  </si>
+  <si>
+    <t>Kidney specific Gene</t>
+  </si>
+  <si>
+    <t>AMACR</t>
+  </si>
+  <si>
+    <t>LRP2</t>
+  </si>
+  <si>
+    <t>ABCG2</t>
+  </si>
+  <si>
+    <t>negative 0.42</t>
+  </si>
+  <si>
+    <t>0.8754</t>
+  </si>
+  <si>
+    <t>negative 0.24</t>
+  </si>
+  <si>
+    <t>their common is type of tissue</t>
+  </si>
+  <si>
+    <t>Bone Marrow specific Gene</t>
+  </si>
+  <si>
+    <t>PRIM2</t>
+  </si>
+  <si>
+    <t>TRFC</t>
+  </si>
+  <si>
+    <t>HMBS</t>
+  </si>
+  <si>
+    <t>E2F8</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>0.7061</t>
+  </si>
+  <si>
+    <t>Placenta specific Gene</t>
+  </si>
+  <si>
+    <t>MGAT4A</t>
+  </si>
+  <si>
+    <t>SHISA3</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>0.92</t>
   </si>
 </sst>
 </file>
@@ -869,7 +971,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,6 +987,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,12 +1036,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1226,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1241,9 +1374,17 @@
     <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1301,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1330,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1359,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1388,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1416,8 +1557,11 @@
       <c r="I6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="O6" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1445,8 +1589,32 @@
       <c r="I7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L7" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1474,8 +1642,32 @@
       <c r="I8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L8" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1503,8 +1695,32 @@
       <c r="I9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L9" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1532,8 +1748,32 @@
       <c r="I10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L10" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1561,8 +1801,28 @@
       <c r="I11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L11" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1590,8 +1850,22 @@
       <c r="I12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L12" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1620,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1649,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1678,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2238,7 +2512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>